<commit_message>
Edit `course-work` in `operation-research`
</commit_message>
<xml_diff>
--- a/3-course-6-semester/operations-research/course-work/Бронников ПМ-1901 - Курсовая работа.xlsx
+++ b/3-course-6-semester/operations-research/course-work/Бронников ПМ-1901 - Курсовая работа.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bronn\Documents\github\university\3-course-6-semester\operations-research\course-work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2555725B-393B-41CE-B758-409A95B3987E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{524427BE-7E86-41C3-92CE-79F374E72F6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Рюкзак" sheetId="1" r:id="rId1"/>
@@ -111,7 +111,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="38">
   <si>
     <t>Задача о рюкзаке</t>
   </si>
@@ -212,20 +212,39 @@
     <t>r(t)</t>
   </si>
   <si>
-    <t>S(t)</t>
-  </si>
-  <si>
     <t>P</t>
   </si>
   <si>
-    <t>a(t)</t>
+    <t>u(t)</t>
+  </si>
+  <si>
+    <t>s(t)</t>
+  </si>
+  <si>
+    <r>
+      <t>F</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>n</t>
+    </r>
+  </si>
+  <si>
+    <t>Матрица функции Беллмана</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -276,8 +295,32 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -326,8 +369,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="43">
+  <borders count="55">
     <border>
       <left/>
       <right/>
@@ -895,11 +944,167 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1012,11 +1217,61 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="44" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="49" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="52" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="53" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1032,6 +1287,61 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>8659</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>4330</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>246784</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Прямая соединительная линия 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB8EA844-AEAF-DC4F-B436-7B2654F419A6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="749011" y="1736148"/>
+          <a:ext cx="484909" cy="415636"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1300,7 +1610,7 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1554,8 +1864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C437A2DE-9EA0-457A-A6EA-CA990C889876}">
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1933,131 +2243,783 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{142A7C0C-BB28-46D8-976D-B40E542371AE}">
-  <dimension ref="B2:L5"/>
+  <dimension ref="D4:R21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T23" sqref="T23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="3.7109375" style="64"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="64" t="s">
+    <row r="4" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D4" s="70" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="64">
+      <c r="E4" s="70">
         <v>0</v>
       </c>
-      <c r="D2" s="64">
+      <c r="F4" s="70">
         <v>1</v>
       </c>
-      <c r="E2" s="64">
+      <c r="G4" s="70">
         <v>2</v>
       </c>
-      <c r="F2" s="64">
+      <c r="H4" s="70">
         <v>3</v>
       </c>
-      <c r="G2" s="64">
+      <c r="I4" s="70">
         <v>4</v>
       </c>
-      <c r="H2" s="64">
+      <c r="J4" s="70">
         <v>5</v>
       </c>
-      <c r="I2" s="64">
+      <c r="K4" s="70">
         <v>6</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L4" s="70">
+        <v>7</v>
+      </c>
+      <c r="M4" s="70">
+        <v>8</v>
+      </c>
+      <c r="N4" s="70">
+        <v>9</v>
+      </c>
+      <c r="O4" s="70">
+        <v>10</v>
+      </c>
+      <c r="Q4" s="64" t="s">
+        <v>35</v>
+      </c>
+      <c r="R4" s="64">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D5" s="70" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="70">
+        <v>31</v>
+      </c>
+      <c r="F5" s="70">
+        <v>30</v>
+      </c>
+      <c r="G5" s="70">
+        <v>28</v>
+      </c>
+      <c r="H5" s="70">
+        <v>28</v>
+      </c>
+      <c r="I5" s="70">
+        <v>27</v>
+      </c>
+      <c r="J5" s="70">
+        <v>26</v>
+      </c>
+      <c r="K5" s="70">
+        <v>26</v>
+      </c>
+      <c r="L5" s="70">
+        <v>25</v>
+      </c>
+      <c r="M5" s="70">
+        <v>24</v>
+      </c>
+      <c r="N5" s="70">
+        <v>24</v>
+      </c>
+      <c r="O5" s="70">
+        <v>23</v>
+      </c>
+      <c r="Q5" s="64" t="s">
+        <v>33</v>
+      </c>
+      <c r="R5" s="64">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D6" s="70" t="s">
         <v>34</v>
       </c>
-      <c r="L2">
+      <c r="E6" s="70">
+        <v>8</v>
+      </c>
+      <c r="F6" s="70">
+        <v>9</v>
+      </c>
+      <c r="G6" s="70">
+        <v>9</v>
+      </c>
+      <c r="H6" s="70">
+        <v>10</v>
+      </c>
+      <c r="I6" s="70">
+        <v>10</v>
+      </c>
+      <c r="J6" s="70">
+        <v>10</v>
+      </c>
+      <c r="K6" s="70">
+        <v>11</v>
+      </c>
+      <c r="L6" s="70">
+        <v>12</v>
+      </c>
+      <c r="M6" s="70">
+        <v>14</v>
+      </c>
+      <c r="N6" s="70">
+        <v>17</v>
+      </c>
+      <c r="O6" s="70">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="4:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="4:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D9" s="71" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="72"/>
+      <c r="F9" s="72"/>
+      <c r="G9" s="72"/>
+      <c r="H9" s="72"/>
+      <c r="I9" s="72"/>
+      <c r="J9" s="72"/>
+      <c r="K9" s="72"/>
+      <c r="L9" s="72"/>
+      <c r="M9" s="72"/>
+      <c r="N9" s="72"/>
+      <c r="O9" s="72"/>
+      <c r="P9" s="73"/>
+    </row>
+    <row r="10" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D10" s="65"/>
+      <c r="E10" s="66" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="74">
+        <v>0</v>
+      </c>
+      <c r="G10" s="74">
+        <v>1</v>
+      </c>
+      <c r="H10" s="74">
+        <v>2</v>
+      </c>
+      <c r="I10" s="74">
+        <v>3</v>
+      </c>
+      <c r="J10" s="74">
+        <v>4</v>
+      </c>
+      <c r="K10" s="74">
+        <v>5</v>
+      </c>
+      <c r="L10" s="74">
+        <v>6</v>
+      </c>
+      <c r="M10" s="74">
+        <v>7</v>
+      </c>
+      <c r="N10" s="74">
+        <v>8</v>
+      </c>
+      <c r="O10" s="74">
+        <v>9</v>
+      </c>
+      <c r="P10" s="75">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="4:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="D11" s="67" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="68"/>
+      <c r="F11" s="76"/>
+      <c r="G11" s="76"/>
+      <c r="H11" s="76"/>
+      <c r="I11" s="76"/>
+      <c r="J11" s="76"/>
+      <c r="K11" s="76"/>
+      <c r="L11" s="76"/>
+      <c r="M11" s="76"/>
+      <c r="N11" s="76"/>
+      <c r="O11" s="76"/>
+      <c r="P11" s="77"/>
+    </row>
+    <row r="12" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D12" s="78">
+        <v>10</v>
+      </c>
+      <c r="E12" s="79"/>
+      <c r="F12" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6,E$5-E$6)</f>
+        <v>23</v>
+      </c>
+      <c r="G12" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6,F$5-F$6)</f>
+        <v>21</v>
+      </c>
+      <c r="H12" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6,G$5-G$6)</f>
+        <v>19</v>
+      </c>
+      <c r="I12" s="81">
+        <f>MAX($R$4-$R$5+$E$5-$E$6,H$5-H$6)</f>
+        <v>18</v>
+      </c>
+      <c r="J12" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6,I$5-I$6)</f>
+        <v>17</v>
+      </c>
+      <c r="K12" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6,J$5-J$6)</f>
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B3" s="64" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" s="64">
+      <c r="L12" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6,K$5-K$6)</f>
         <v>15</v>
       </c>
-      <c r="D3" s="64">
-        <v>14</v>
-      </c>
-      <c r="E3" s="64">
+      <c r="M12" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6,L$5-L$6)</f>
         <v>13</v>
       </c>
-      <c r="F3" s="64">
-        <v>13</v>
-      </c>
-      <c r="G3" s="64">
-        <v>12</v>
-      </c>
-      <c r="H3" s="64">
-        <v>12</v>
-      </c>
-      <c r="I3" s="64">
+      <c r="N12" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6,M$5-M$6)</f>
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B4" s="64" t="s">
+      <c r="O12" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6,N$5-N$6)</f>
+        <v>9</v>
+      </c>
+      <c r="P12" s="82">
+        <f>MAX($R$4-$R$5+$E$5-$E$6,O$5-O$6)</f>
+        <v>9</v>
+      </c>
+      <c r="Q12" s="69">
+        <f>$R$4-$R$5+$E$5-$E$6</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D13" s="78">
+        <v>9</v>
+      </c>
+      <c r="E13" s="79"/>
+      <c r="F13" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G$12,E$5-E$6+G12)</f>
+        <v>44</v>
+      </c>
+      <c r="G13" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G$12,F$5-F$6+H12)</f>
+        <v>40</v>
+      </c>
+      <c r="H13" s="81">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G$12,G$5-G$6+I12)</f>
+        <v>37</v>
+      </c>
+      <c r="I13" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G$12,H$5-H$6+J12)</f>
+        <v>35</v>
+      </c>
+      <c r="J13" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G$12,I$5-I$6+K12)</f>
         <v>33</v>
       </c>
-      <c r="C4" s="64">
-        <v>16</v>
-      </c>
-      <c r="D4" s="64">
-        <v>14</v>
-      </c>
-      <c r="E4" s="64">
-        <v>13</v>
-      </c>
-      <c r="F4" s="64">
-        <v>11</v>
-      </c>
-      <c r="G4" s="64">
-        <v>10</v>
-      </c>
-      <c r="H4" s="64">
+      <c r="K13" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G$12,J$5-J$6+L12)</f>
+        <v>31</v>
+      </c>
+      <c r="L13" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G$12,K$5-K$6+M12)</f>
+        <v>30</v>
+      </c>
+      <c r="M13" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G$12,L$5-L$6+N12)</f>
+        <v>30</v>
+      </c>
+      <c r="N13" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G$12,M$5-M$6+O12)</f>
+        <v>30</v>
+      </c>
+      <c r="O13" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G$12,N$5-N$6+P12)</f>
+        <v>30</v>
+      </c>
+      <c r="P13" s="82">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G$12,O$5-O$6+Q12)</f>
+        <v>30</v>
+      </c>
+      <c r="Q13" s="69">
+        <f>$R$4-$R$5+$E$5-$E$6+$G12</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D14" s="78">
         <v>8</v>
       </c>
-      <c r="I4" s="64">
+      <c r="E14" s="79"/>
+      <c r="F14" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G13,E$5-E$6+G13)</f>
+        <v>63</v>
+      </c>
+      <c r="G14" s="81">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G13,F$5-F$6+H13)</f>
+        <v>58</v>
+      </c>
+      <c r="H14" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G13,G$5-G$6+I13)</f>
+        <v>54</v>
+      </c>
+      <c r="I14" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G13,H$5-H$6+J13)</f>
+        <v>51</v>
+      </c>
+      <c r="J14" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G13,I$5-I$6+K13)</f>
+        <v>49</v>
+      </c>
+      <c r="K14" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G13,J$5-J$6+L13)</f>
+        <v>49</v>
+      </c>
+      <c r="L14" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G13,K$5-K$6+M13)</f>
+        <v>49</v>
+      </c>
+      <c r="M14" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G13,L$5-L$6+N13)</f>
+        <v>49</v>
+      </c>
+      <c r="N14" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G13,M$5-M$6+O13)</f>
+        <v>49</v>
+      </c>
+      <c r="O14" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G13,N$5-N$6+P13)</f>
+        <v>49</v>
+      </c>
+      <c r="P14" s="82">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G13,O$5-O$6+Q13)</f>
+        <v>49</v>
+      </c>
+      <c r="Q14" s="69">
+        <f t="shared" ref="Q14:Q21" si="0">$R$4-$R$5+$E$5-$E$6+$G13</f>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D15" s="78">
+        <v>7</v>
+      </c>
+      <c r="E15" s="79"/>
+      <c r="F15" s="81">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G14,E$5-E$6+G14)</f>
+        <v>81</v>
+      </c>
+      <c r="G15" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G14,F$5-F$6+H14)</f>
+        <v>75</v>
+      </c>
+      <c r="H15" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G14,G$5-G$6+I14)</f>
+        <v>70</v>
+      </c>
+      <c r="I15" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G14,H$5-H$6+J14)</f>
+        <v>67</v>
+      </c>
+      <c r="J15" s="83">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G14,I$5-I$6+K14)</f>
+        <v>67</v>
+      </c>
+      <c r="K15" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G14,J$5-J$6+L14)</f>
+        <v>67</v>
+      </c>
+      <c r="L15" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G14,K$5-K$6+M14)</f>
+        <v>67</v>
+      </c>
+      <c r="M15" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G14,L$5-L$6+N14)</f>
+        <v>67</v>
+      </c>
+      <c r="N15" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G14,M$5-M$6+O14)</f>
+        <v>67</v>
+      </c>
+      <c r="O15" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G14,N$5-N$6+P14)</f>
+        <v>67</v>
+      </c>
+      <c r="P15" s="82">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G14,O$5-O$6+Q14)</f>
+        <v>67</v>
+      </c>
+      <c r="Q15" s="69">
+        <f t="shared" si="0"/>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D16" s="78">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="65" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5" s="66" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="64">
-        <f t="shared" ref="D5:I5" si="0">D4-$L$2+$C$3</f>
-        <v>13</v>
-      </c>
-      <c r="E5" s="64">
+      <c r="E16" s="79"/>
+      <c r="F16" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G15,E$5-E$6+G15)</f>
+        <v>98</v>
+      </c>
+      <c r="G16" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G15,F$5-F$6+H15)</f>
+        <v>91</v>
+      </c>
+      <c r="H16" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G15,G$5-G$6+I15)</f>
+        <v>86</v>
+      </c>
+      <c r="I16" s="81">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G15,H$5-H$6+J15)</f>
+        <v>85</v>
+      </c>
+      <c r="J16" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G15,I$5-I$6+K15)</f>
+        <v>84</v>
+      </c>
+      <c r="K16" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G15,J$5-J$6+L15)</f>
+        <v>84</v>
+      </c>
+      <c r="L16" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G15,K$5-K$6+M15)</f>
+        <v>84</v>
+      </c>
+      <c r="M16" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G15,L$5-L$6+N15)</f>
+        <v>84</v>
+      </c>
+      <c r="N16" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G15,M$5-M$6+O15)</f>
+        <v>84</v>
+      </c>
+      <c r="O16" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G15,N$5-N$6+P15)</f>
+        <v>84</v>
+      </c>
+      <c r="P16" s="82">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G15,O$5-O$6+Q15)</f>
+        <v>84</v>
+      </c>
+      <c r="Q16" s="69">
         <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="F5" s="64">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D17" s="78">
+        <v>5</v>
+      </c>
+      <c r="E17" s="79"/>
+      <c r="F17" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G16,E$5-E$6+G16)</f>
+        <v>114</v>
+      </c>
+      <c r="G17" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G16,F$5-F$6+H16)</f>
+        <v>107</v>
+      </c>
+      <c r="H17" s="81">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G16,G$5-G$6+I16)</f>
+        <v>104</v>
+      </c>
+      <c r="I17" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G16,H$5-H$6+J16)</f>
+        <v>102</v>
+      </c>
+      <c r="J17" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G16,I$5-I$6+K16)</f>
+        <v>101</v>
+      </c>
+      <c r="K17" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G16,J$5-J$6+L16)</f>
+        <v>100</v>
+      </c>
+      <c r="L17" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G16,K$5-K$6+M16)</f>
+        <v>100</v>
+      </c>
+      <c r="M17" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G16,L$5-L$6+N16)</f>
+        <v>100</v>
+      </c>
+      <c r="N17" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G16,M$5-M$6+O16)</f>
+        <v>100</v>
+      </c>
+      <c r="O17" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G16,N$5-N$6+P16)</f>
+        <v>100</v>
+      </c>
+      <c r="P17" s="82">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G16,O$5-O$6+Q16)</f>
+        <v>100</v>
+      </c>
+      <c r="Q17" s="69">
         <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="G5" s="64">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D18" s="78">
+        <v>4</v>
+      </c>
+      <c r="E18" s="79"/>
+      <c r="F18" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G17,E$5-E$6+G17)</f>
+        <v>130</v>
+      </c>
+      <c r="G18" s="81">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G17,F$5-F$6+H17)</f>
+        <v>125</v>
+      </c>
+      <c r="H18" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G17,G$5-G$6+I17)</f>
+        <v>121</v>
+      </c>
+      <c r="I18" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G17,H$5-H$6+J17)</f>
+        <v>119</v>
+      </c>
+      <c r="J18" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G17,I$5-I$6+K17)</f>
+        <v>117</v>
+      </c>
+      <c r="K18" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G17,J$5-J$6+L17)</f>
+        <v>116</v>
+      </c>
+      <c r="L18" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G17,K$5-K$6+M17)</f>
+        <v>116</v>
+      </c>
+      <c r="M18" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G17,L$5-L$6+N17)</f>
+        <v>116</v>
+      </c>
+      <c r="N18" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G17,M$5-M$6+O17)</f>
+        <v>116</v>
+      </c>
+      <c r="O18" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G17,N$5-N$6+P17)</f>
+        <v>116</v>
+      </c>
+      <c r="P18" s="82">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G17,O$5-O$6+Q17)</f>
+        <v>116</v>
+      </c>
+      <c r="Q18" s="69">
         <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="H5" s="64">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="19" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D19" s="78">
+        <v>3</v>
+      </c>
+      <c r="E19" s="79"/>
+      <c r="F19" s="81">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G18,E$5-E$6+G18)</f>
+        <v>148</v>
+      </c>
+      <c r="G19" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G18,F$5-F$6+H18)</f>
+        <v>142</v>
+      </c>
+      <c r="H19" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G18,G$5-G$6+I18)</f>
+        <v>138</v>
+      </c>
+      <c r="I19" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G18,H$5-H$6+J18)</f>
+        <v>135</v>
+      </c>
+      <c r="J19" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G18,I$5-I$6+K18)</f>
+        <v>134</v>
+      </c>
+      <c r="K19" s="83">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G18,J$5-J$6+L18)</f>
+        <v>134</v>
+      </c>
+      <c r="L19" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G18,K$5-K$6+M18)</f>
+        <v>134</v>
+      </c>
+      <c r="M19" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G18,L$5-L$6+N18)</f>
+        <v>134</v>
+      </c>
+      <c r="N19" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G18,M$5-M$6+O18)</f>
+        <v>134</v>
+      </c>
+      <c r="O19" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G18,N$5-N$6+P18)</f>
+        <v>134</v>
+      </c>
+      <c r="P19" s="82">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G18,O$5-O$6+Q18)</f>
+        <v>134</v>
+      </c>
+      <c r="Q19" s="69">
         <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="I5" s="64">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="20" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D20" s="78">
+        <v>2</v>
+      </c>
+      <c r="E20" s="79"/>
+      <c r="F20" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G19,E$5-E$6+G19)</f>
+        <v>165</v>
+      </c>
+      <c r="G20" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G19,F$5-F$6+H19)</f>
+        <v>159</v>
+      </c>
+      <c r="H20" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G19,G$5-G$6+I19)</f>
+        <v>154</v>
+      </c>
+      <c r="I20" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G19,H$5-H$6+J19)</f>
+        <v>152</v>
+      </c>
+      <c r="J20" s="81">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G19,I$5-I$6+K19)</f>
+        <v>151</v>
+      </c>
+      <c r="K20" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G19,J$5-J$6+L19)</f>
+        <v>151</v>
+      </c>
+      <c r="L20" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G19,K$5-K$6+M19)</f>
+        <v>151</v>
+      </c>
+      <c r="M20" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G19,L$5-L$6+N19)</f>
+        <v>151</v>
+      </c>
+      <c r="N20" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G19,M$5-M$6+O19)</f>
+        <v>151</v>
+      </c>
+      <c r="O20" s="80">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G19,N$5-N$6+P19)</f>
+        <v>151</v>
+      </c>
+      <c r="P20" s="82">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G19,O$5-O$6+Q19)</f>
+        <v>151</v>
+      </c>
+      <c r="Q20" s="69">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>151</v>
+      </c>
+    </row>
+    <row r="21" spans="4:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D21" s="84">
+        <v>1</v>
+      </c>
+      <c r="E21" s="85"/>
+      <c r="F21" s="86">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G20,E$5-E$6+G20)</f>
+        <v>182</v>
+      </c>
+      <c r="G21" s="86">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G20,F$5-F$6+H20)</f>
+        <v>175</v>
+      </c>
+      <c r="H21" s="86">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G20,G$5-G$6+I20)</f>
+        <v>171</v>
+      </c>
+      <c r="I21" s="87">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G20,H$5-H$6+J20)</f>
+        <v>169</v>
+      </c>
+      <c r="J21" s="86">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G20,I$5-I$6+K20)</f>
+        <v>168</v>
+      </c>
+      <c r="K21" s="86">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G20,J$5-J$6+L20)</f>
+        <v>168</v>
+      </c>
+      <c r="L21" s="86">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G20,K$5-K$6+M20)</f>
+        <v>168</v>
+      </c>
+      <c r="M21" s="86">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G20,L$5-L$6+N20)</f>
+        <v>168</v>
+      </c>
+      <c r="N21" s="86">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G20,M$5-M$6+O20)</f>
+        <v>168</v>
+      </c>
+      <c r="O21" s="86">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G20,N$5-N$6+P20)</f>
+        <v>168</v>
+      </c>
+      <c r="P21" s="88">
+        <f>MAX($R$4-$R$5+$E$5-$E$6+$G20,O$5-O$6+Q20)</f>
+        <v>168</v>
+      </c>
+      <c r="Q21" s="69">
+        <f t="shared" si="0"/>
+        <v>168</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="22">
+    <mergeCell ref="M10:M11"/>
+    <mergeCell ref="N10:N11"/>
+    <mergeCell ref="O10:O11"/>
+    <mergeCell ref="P10:P11"/>
+    <mergeCell ref="D9:P9"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="I10:I11"/>
+    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="K10:K11"/>
+    <mergeCell ref="L10:L11"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>